<commit_message>
Solved : SURF, SIFT; Issues: Random Forest
</commit_message>
<xml_diff>
--- a/Lab4/SIFT Train Results.xlsx
+++ b/Lab4/SIFT Train Results.xlsx
@@ -11,6 +11,161 @@
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+  <si>
+    <t>apple2-090-090.png</t>
+  </si>
+  <si>
+    <t>apple2-090-112.png</t>
+  </si>
+  <si>
+    <t>apple2-090-135.png</t>
+  </si>
+  <si>
+    <t>apple2-090-158.png</t>
+  </si>
+  <si>
+    <t>apple2-090-180.png</t>
+  </si>
+  <si>
+    <t>apple2-090-202.png</t>
+  </si>
+  <si>
+    <t>apple2-090-225.png</t>
+  </si>
+  <si>
+    <t>apple2-090-248.png</t>
+  </si>
+  <si>
+    <t>apple2-090-270.png</t>
+  </si>
+  <si>
+    <t>apple2-090-292.png</t>
+  </si>
+  <si>
+    <t>apple2-090-315.png</t>
+  </si>
+  <si>
+    <t>apple2-090-338.png</t>
+  </si>
+  <si>
+    <t>apple3-000-000.png</t>
+  </si>
+  <si>
+    <t>apple3-022-000.png</t>
+  </si>
+  <si>
+    <t>apple3-022-090.png</t>
+  </si>
+  <si>
+    <t>apple3-022-180.png</t>
+  </si>
+  <si>
+    <t>apple3-022-270.png</t>
+  </si>
+  <si>
+    <t>apple3-035-045.png</t>
+  </si>
+  <si>
+    <t>apple3-035-135.png</t>
+  </si>
+  <si>
+    <t>apple3-035-225.png</t>
+  </si>
+  <si>
+    <t>apple9-022-090.png</t>
+  </si>
+  <si>
+    <t>apple9-022-180.png</t>
+  </si>
+  <si>
+    <t>apple9-022-270.png</t>
+  </si>
+  <si>
+    <t>apple9-035-045.png</t>
+  </si>
+  <si>
+    <t>apple9-035-135.png</t>
+  </si>
+  <si>
+    <t>apple9-035-225.png</t>
+  </si>
+  <si>
+    <t>apple9-035-315.png</t>
+  </si>
+  <si>
+    <t>apple9-045-000.png</t>
+  </si>
+  <si>
+    <t>apple9-045-090.png</t>
+  </si>
+  <si>
+    <t>apple9-045-180.png</t>
+  </si>
+  <si>
+    <t>car2-090-112.png</t>
+  </si>
+  <si>
+    <t>car2-090-135.png</t>
+  </si>
+  <si>
+    <t>car2-090-158.png</t>
+  </si>
+  <si>
+    <t>car2-090-180.png</t>
+  </si>
+  <si>
+    <t>car2-090-202.png</t>
+  </si>
+  <si>
+    <t>car2-090-225.png</t>
+  </si>
+  <si>
+    <t>car2-090-248.png</t>
+  </si>
+  <si>
+    <t>car2-090-270.png</t>
+  </si>
+  <si>
+    <t>car2-090-292.png</t>
+  </si>
+  <si>
+    <t>car2-090-315.png</t>
+  </si>
+  <si>
+    <t>car2-090-338.png</t>
+  </si>
+  <si>
+    <t>car3-000-000.png</t>
+  </si>
+  <si>
+    <t>car3-022-000.png</t>
+  </si>
+  <si>
+    <t>car3-022-090.png</t>
+  </si>
+  <si>
+    <t>car3-022-180.png</t>
+  </si>
+  <si>
+    <t>car3-022-270.png</t>
+  </si>
+  <si>
+    <t>car3-035-045.png</t>
+  </si>
+  <si>
+    <t>car3-035-135.png</t>
+  </si>
+  <si>
+    <t>car3-035-225.png</t>
+  </si>
+  <si>
+    <t>car3-035-315.png</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -340,93 +495,96 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:T52"/>
+  <dimension ref="A3:U52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="3" spans="1:20">
-      <c r="A3">
+    <row r="3" spans="1:21">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
         <v>55</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>85</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>44</v>
       </c>
-      <c r="F3">
-        <v>3</v>
-      </c>
       <c r="G3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J3">
         <v>2</v>
       </c>
       <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3">
         <v>20</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>52</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>82</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>18</v>
       </c>
-      <c r="O3">
-        <v>2</v>
-      </c>
       <c r="P3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
         <v>9</v>
       </c>
-      <c r="R3">
-        <v>3</v>
-      </c>
       <c r="S3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T3">
+        <v>2</v>
+      </c>
+      <c r="U3">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
-      <c r="A4">
+    <row r="4" spans="1:21">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
         <v>18</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
         <v>6</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>74</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
       <c r="G4">
         <v>0</v>
       </c>
@@ -434,107 +592,113 @@
         <v>0</v>
       </c>
       <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
         <v>184</v>
       </c>
-      <c r="J4">
-        <v>2</v>
-      </c>
       <c r="K4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
         <v>11</v>
       </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
         <v>12</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>151</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>7</v>
       </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
       <c r="T4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:20">
-      <c r="A5">
+      <c r="U4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
         <v>24</v>
       </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
       <c r="C5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
         <v>8</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>110</v>
       </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
       <c r="G5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
         <v>179</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>18</v>
       </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
       <c r="L5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M5">
+        <v>2</v>
+      </c>
+      <c r="N5">
         <v>14</v>
       </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
         <v>120</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>14</v>
       </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
       <c r="T5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:20">
-      <c r="A6">
-        <v>0</v>
+      <c r="U5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
+      <c r="A6" t="s">
+        <v>3</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -546,63 +710,66 @@
         <v>0</v>
       </c>
       <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
         <v>22</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>14</v>
       </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
         <v>5</v>
       </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
       <c r="K6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
         <v>71</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>23</v>
       </c>
-      <c r="O6">
-        <v>2</v>
-      </c>
       <c r="P6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q6">
+        <v>3</v>
+      </c>
+      <c r="R6">
         <v>64</v>
       </c>
-      <c r="R6">
-        <v>1</v>
-      </c>
       <c r="S6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:20">
-      <c r="A7">
+      <c r="U6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
         <v>35</v>
       </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
       <c r="C7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -617,14 +784,14 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7">
         <v>168</v>
       </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
       <c r="K7">
         <v>0</v>
       </c>
@@ -641,27 +808,30 @@
         <v>0</v>
       </c>
       <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
         <v>29</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>168</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <v>7</v>
       </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
       <c r="T7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:20">
-      <c r="A8">
-        <v>2</v>
+      <c r="U7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
+      <c r="A8" t="s">
+        <v>5</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -676,17 +846,17 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I8">
+        <v>2</v>
+      </c>
+      <c r="J8">
         <v>57</v>
       </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
       <c r="K8">
         <v>0</v>
       </c>
@@ -703,28 +873,31 @@
         <v>0</v>
       </c>
       <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
         <v>25</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <v>189</v>
       </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
       <c r="S8">
         <v>0</v>
       </c>
       <c r="T8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:20">
-      <c r="A9">
+      <c r="U8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
         <v>26</v>
       </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
       <c r="C9">
         <v>0</v>
       </c>
@@ -738,17 +911,17 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9">
         <v>6</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>178</v>
       </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
       <c r="K9">
         <v>0</v>
       </c>
@@ -765,30 +938,33 @@
         <v>0</v>
       </c>
       <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
         <v>37</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>178</v>
       </c>
-      <c r="R9">
-        <v>3</v>
-      </c>
       <c r="S9">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:20">
-      <c r="A10">
-        <v>1</v>
+      <c r="U9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
+      <c r="A10" t="s">
+        <v>7</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -797,25 +973,25 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
         <v>57</v>
       </c>
-      <c r="J10">
-        <v>3</v>
-      </c>
       <c r="K10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M10">
         <v>0</v>
@@ -827,24 +1003,27 @@
         <v>0</v>
       </c>
       <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
         <v>17</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>153</v>
       </c>
-      <c r="R10">
-        <v>2</v>
-      </c>
       <c r="S10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:20">
-      <c r="A11">
-        <v>0</v>
+      <c r="U10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
+      <c r="A11" t="s">
+        <v>8</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -853,69 +1032,72 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
         <v>142</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>16</v>
       </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
         <v>80</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>10</v>
       </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
       <c r="L11">
         <v>0</v>
       </c>
       <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
         <v>142</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <v>34</v>
       </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
       <c r="P11">
         <v>0</v>
       </c>
       <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
         <v>142</v>
       </c>
-      <c r="R11">
+      <c r="S11">
         <v>38</v>
       </c>
-      <c r="S11">
-        <v>0</v>
-      </c>
       <c r="T11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:20">
-      <c r="A12">
+      <c r="U11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
         <v>44</v>
       </c>
-      <c r="B12">
-        <v>3</v>
-      </c>
       <c r="C12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -927,14 +1109,14 @@
         <v>0</v>
       </c>
       <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
         <v>6</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>180</v>
       </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
       <c r="K12">
         <v>0</v>
       </c>
@@ -951,24 +1133,27 @@
         <v>0</v>
       </c>
       <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
         <v>40</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <v>180</v>
       </c>
-      <c r="R12">
+      <c r="S12">
         <v>15</v>
       </c>
-      <c r="S12">
-        <v>0</v>
-      </c>
       <c r="T12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:20">
-      <c r="A13">
-        <v>0</v>
+      <c r="U12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
+      <c r="A13" t="s">
+        <v>10</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -980,63 +1165,66 @@
         <v>0</v>
       </c>
       <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
         <v>82</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>61</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>5</v>
       </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
       <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
         <v>48</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>13</v>
       </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
       <c r="L13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
         <v>137</v>
       </c>
-      <c r="N13">
+      <c r="O13">
         <v>38</v>
       </c>
-      <c r="O13">
-        <v>0</v>
-      </c>
       <c r="P13">
         <v>0</v>
       </c>
       <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
         <v>137</v>
       </c>
-      <c r="R13">
+      <c r="S13">
         <v>41</v>
       </c>
-      <c r="S13">
-        <v>0</v>
-      </c>
       <c r="T13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:20">
-      <c r="A14">
+      <c r="U13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
         <v>48</v>
       </c>
-      <c r="B14">
-        <v>2</v>
-      </c>
       <c r="C14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -1051,16 +1239,16 @@
         <v>0</v>
       </c>
       <c r="H14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
         <v>187</v>
       </c>
-      <c r="J14">
-        <v>2</v>
-      </c>
       <c r="K14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L14">
         <v>0</v>
@@ -1075,116 +1263,122 @@
         <v>0</v>
       </c>
       <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
         <v>5</v>
       </c>
-      <c r="Q14">
+      <c r="R14">
         <v>148</v>
       </c>
-      <c r="R14">
-        <v>3</v>
-      </c>
       <c r="S14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:20">
-      <c r="A15">
-        <v>0</v>
+      <c r="U14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21">
+      <c r="A15" t="s">
+        <v>12</v>
       </c>
       <c r="B15">
         <v>0</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
         <v>8</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>15</v>
       </c>
-      <c r="G15">
-        <v>3</v>
-      </c>
       <c r="H15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
         <v>98</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>7</v>
       </c>
-      <c r="K15">
-        <v>1</v>
-      </c>
       <c r="L15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P15">
+        <v>3</v>
+      </c>
+      <c r="Q15">
         <v>12</v>
       </c>
-      <c r="Q15">
+      <c r="R15">
         <v>185</v>
       </c>
-      <c r="R15">
-        <v>3</v>
-      </c>
       <c r="S15">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:20">
-      <c r="A16">
-        <v>2</v>
+      <c r="U15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21">
+      <c r="A16" t="s">
+        <v>13</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="F16">
         <v>5</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>11</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>4</v>
       </c>
-      <c r="H16">
-        <v>3</v>
-      </c>
       <c r="I16">
+        <v>3</v>
+      </c>
+      <c r="J16">
         <v>87</v>
       </c>
-      <c r="J16">
-        <v>3</v>
-      </c>
       <c r="K16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L16">
         <v>0</v>
@@ -1193,30 +1387,33 @@
         <v>0</v>
       </c>
       <c r="N16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O16">
+        <v>2</v>
+      </c>
+      <c r="P16">
         <v>4</v>
       </c>
-      <c r="P16">
+      <c r="Q16">
         <v>10</v>
       </c>
-      <c r="Q16">
+      <c r="R16">
         <v>187</v>
       </c>
-      <c r="R16">
+      <c r="S16">
         <v>4</v>
       </c>
-      <c r="S16">
-        <v>0</v>
-      </c>
       <c r="T16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:20">
-      <c r="A17">
-        <v>1</v>
+      <c r="U16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21">
+      <c r="A17" t="s">
+        <v>14</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -1225,93 +1422,96 @@
         <v>1</v>
       </c>
       <c r="D17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="G17">
         <v>9</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>4</v>
       </c>
-      <c r="H17">
-        <v>1</v>
-      </c>
       <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
         <v>46</v>
       </c>
-      <c r="J17">
-        <v>3</v>
-      </c>
       <c r="K17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L17">
         <v>1</v>
       </c>
       <c r="M17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N17">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O17">
+        <v>3</v>
+      </c>
+      <c r="P17">
         <v>10</v>
       </c>
-      <c r="P17">
+      <c r="Q17">
         <v>15</v>
       </c>
-      <c r="Q17">
+      <c r="R17">
         <v>184</v>
       </c>
-      <c r="R17">
-        <v>1</v>
-      </c>
       <c r="S17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:20">
-      <c r="A18">
+      <c r="U17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18">
         <v>5</v>
       </c>
-      <c r="B18">
+      <c r="C18">
         <v>8</v>
       </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
       <c r="D18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
         <v>4</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>8</v>
       </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
       <c r="H18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
         <v>93</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <v>7</v>
       </c>
-      <c r="K18">
-        <v>1</v>
-      </c>
       <c r="L18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M18">
         <v>0</v>
@@ -1320,117 +1520,123 @@
         <v>0</v>
       </c>
       <c r="O18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P18">
+        <v>1</v>
+      </c>
+      <c r="Q18">
         <v>10</v>
       </c>
-      <c r="Q18">
+      <c r="R18">
         <v>183</v>
       </c>
-      <c r="R18">
-        <v>1</v>
-      </c>
       <c r="S18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:20">
-      <c r="A19">
+      <c r="U18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19">
         <v>7</v>
       </c>
-      <c r="B19">
+      <c r="C19">
         <v>4</v>
       </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
       <c r="D19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H19">
+        <v>3</v>
+      </c>
+      <c r="I19">
         <v>4</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>77</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>9</v>
       </c>
-      <c r="K19">
-        <v>1</v>
-      </c>
       <c r="L19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
         <v>14</v>
       </c>
-      <c r="Q19">
+      <c r="R19">
         <v>186</v>
       </c>
-      <c r="R19">
-        <v>2</v>
-      </c>
       <c r="S19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:20">
-      <c r="A20">
-        <v>1</v>
+      <c r="U19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21">
+      <c r="A20" t="s">
+        <v>17</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20">
         <v>0</v>
       </c>
       <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
         <v>5</v>
       </c>
-      <c r="E20">
-        <v>3</v>
-      </c>
       <c r="F20">
         <v>3</v>
       </c>
       <c r="G20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H20">
         <v>2</v>
       </c>
       <c r="I20">
+        <v>2</v>
+      </c>
+      <c r="J20">
         <v>81</v>
       </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
       <c r="K20">
         <v>0</v>
       </c>
@@ -1441,101 +1647,107 @@
         <v>0</v>
       </c>
       <c r="N20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P20">
+        <v>3</v>
+      </c>
+      <c r="Q20">
         <v>23</v>
       </c>
-      <c r="Q20">
+      <c r="R20">
         <v>184</v>
       </c>
-      <c r="R20">
-        <v>0</v>
-      </c>
       <c r="S20">
         <v>0</v>
       </c>
       <c r="T20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:20">
-      <c r="A21">
-        <v>1</v>
+      <c r="U20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21">
+      <c r="A21" t="s">
+        <v>18</v>
       </c>
       <c r="B21">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21">
         <v>4</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>6</v>
       </c>
-      <c r="F21">
-        <v>3</v>
-      </c>
       <c r="G21">
+        <v>3</v>
+      </c>
+      <c r="H21">
         <v>7</v>
       </c>
-      <c r="H21">
-        <v>3</v>
-      </c>
       <c r="I21">
+        <v>3</v>
+      </c>
+      <c r="J21">
         <v>58</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <v>9</v>
       </c>
-      <c r="K21">
+      <c r="L21">
         <v>8</v>
       </c>
-      <c r="L21">
-        <v>2</v>
-      </c>
       <c r="M21">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N21">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O21">
+        <v>2</v>
+      </c>
+      <c r="P21">
         <v>4</v>
       </c>
-      <c r="P21">
+      <c r="Q21">
         <v>9</v>
       </c>
-      <c r="Q21">
+      <c r="R21">
         <v>174</v>
       </c>
-      <c r="R21">
-        <v>3</v>
-      </c>
       <c r="S21">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="T21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20">
-      <c r="A22">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="U21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21">
+      <c r="A22" t="s">
+        <v>19</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E22">
         <v>2</v>
@@ -1544,17 +1756,17 @@
         <v>2</v>
       </c>
       <c r="G22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I22">
+        <v>2</v>
+      </c>
+      <c r="J22">
         <v>60</v>
       </c>
-      <c r="J22">
-        <v>0</v>
-      </c>
       <c r="K22">
         <v>0</v>
       </c>
@@ -1562,101 +1774,107 @@
         <v>0</v>
       </c>
       <c r="M22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O22">
         <v>2</v>
       </c>
       <c r="P22">
+        <v>2</v>
+      </c>
+      <c r="Q22">
         <v>15</v>
       </c>
-      <c r="Q22">
+      <c r="R22">
         <v>190</v>
       </c>
-      <c r="R22">
-        <v>0</v>
-      </c>
       <c r="S22">
         <v>0</v>
       </c>
       <c r="T22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:20">
-      <c r="A23">
+      <c r="U22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23">
         <v>8</v>
       </c>
-      <c r="B23">
+      <c r="C23">
         <v>5</v>
       </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
       <c r="D23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H23">
         <v>1</v>
       </c>
       <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23">
         <v>95</v>
       </c>
-      <c r="J23">
-        <v>1</v>
-      </c>
       <c r="K23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M23">
+        <v>1</v>
+      </c>
+      <c r="N23">
         <v>4</v>
       </c>
-      <c r="N23">
-        <v>3</v>
-      </c>
       <c r="O23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P23">
+        <v>1</v>
+      </c>
+      <c r="Q23">
         <v>5</v>
       </c>
-      <c r="Q23">
+      <c r="R23">
         <v>196</v>
       </c>
-      <c r="R23">
-        <v>0</v>
-      </c>
       <c r="S23">
         <v>0</v>
       </c>
       <c r="T23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:20">
-      <c r="A24">
+      <c r="U23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24">
         <v>51</v>
       </c>
-      <c r="B24">
-        <v>2</v>
-      </c>
       <c r="C24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -1665,23 +1883,23 @@
         <v>0</v>
       </c>
       <c r="F24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H24">
+        <v>2</v>
+      </c>
+      <c r="I24">
         <v>7</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>181</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <v>5</v>
       </c>
-      <c r="K24">
-        <v>0</v>
-      </c>
       <c r="L24">
         <v>0</v>
       </c>
@@ -1695,24 +1913,27 @@
         <v>0</v>
       </c>
       <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24">
         <v>21</v>
       </c>
-      <c r="Q24">
+      <c r="R24">
         <v>149</v>
       </c>
-      <c r="R24">
+      <c r="S24">
         <v>5</v>
       </c>
-      <c r="S24">
-        <v>0</v>
-      </c>
       <c r="T24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:20">
-      <c r="A25">
-        <v>0</v>
+      <c r="U24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21">
+      <c r="A25" t="s">
+        <v>22</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -1721,153 +1942,159 @@
         <v>0</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25">
         <v>1</v>
       </c>
       <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
         <v>6</v>
       </c>
-      <c r="G25">
-        <v>3</v>
-      </c>
       <c r="H25">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25">
         <v>96</v>
       </c>
-      <c r="J25">
-        <v>2</v>
-      </c>
       <c r="K25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L25">
         <v>0</v>
       </c>
       <c r="M25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N25">
+        <v>1</v>
+      </c>
+      <c r="O25">
         <v>5</v>
       </c>
-      <c r="O25">
-        <v>1</v>
-      </c>
       <c r="P25">
+        <v>1</v>
+      </c>
+      <c r="Q25">
         <v>12</v>
       </c>
-      <c r="Q25">
+      <c r="R25">
         <v>204</v>
       </c>
-      <c r="R25">
-        <v>0</v>
-      </c>
       <c r="S25">
         <v>0</v>
       </c>
       <c r="T25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:20">
-      <c r="A26">
-        <v>1</v>
+      <c r="U25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21">
+      <c r="A26" t="s">
+        <v>23</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F26">
+        <v>3</v>
+      </c>
+      <c r="G26">
         <v>4</v>
       </c>
-      <c r="G26">
-        <v>3</v>
-      </c>
       <c r="H26">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26">
         <v>120</v>
       </c>
-      <c r="J26">
+      <c r="K26">
         <v>20</v>
       </c>
-      <c r="K26">
-        <v>1</v>
-      </c>
       <c r="L26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O26">
         <v>0</v>
       </c>
       <c r="P26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q26">
+        <v>1</v>
+      </c>
+      <c r="R26">
         <v>173</v>
       </c>
-      <c r="R26">
+      <c r="S26">
         <v>30</v>
       </c>
-      <c r="S26">
-        <v>0</v>
-      </c>
       <c r="T26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:20">
-      <c r="A27">
-        <v>6</v>
+      <c r="U26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21">
+      <c r="A27" t="s">
+        <v>24</v>
       </c>
       <c r="B27">
         <v>6</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27">
         <v>0</v>
       </c>
       <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
         <v>7</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <v>6</v>
       </c>
-      <c r="H27">
-        <v>1</v>
-      </c>
       <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27">
         <v>126</v>
       </c>
-      <c r="J27">
+      <c r="K27">
         <v>10</v>
       </c>
-      <c r="K27">
-        <v>0</v>
-      </c>
       <c r="L27">
         <v>0</v>
       </c>
@@ -1881,39 +2108,42 @@
         <v>0</v>
       </c>
       <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
         <v>7</v>
       </c>
-      <c r="Q27">
+      <c r="R27">
         <v>189</v>
       </c>
-      <c r="R27">
+      <c r="S27">
         <v>9</v>
       </c>
-      <c r="S27">
-        <v>0</v>
-      </c>
       <c r="T27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:20">
-      <c r="A28">
-        <v>2</v>
+      <c r="U27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21">
+      <c r="A28" t="s">
+        <v>25</v>
       </c>
       <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28">
         <v>4</v>
       </c>
-      <c r="C28">
-        <v>3</v>
-      </c>
       <c r="D28">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E28">
         <v>2</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G28">
         <v>0</v>
@@ -1922,19 +2152,19 @@
         <v>0</v>
       </c>
       <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
         <v>85</v>
       </c>
-      <c r="J28">
+      <c r="K28">
         <v>5</v>
       </c>
-      <c r="K28">
-        <v>3</v>
-      </c>
       <c r="L28">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N28">
         <v>0</v>
@@ -1943,34 +2173,37 @@
         <v>0</v>
       </c>
       <c r="P28">
+        <v>0</v>
+      </c>
+      <c r="Q28">
         <v>7</v>
       </c>
-      <c r="Q28">
+      <c r="R28">
         <v>198</v>
       </c>
-      <c r="R28">
-        <v>2</v>
-      </c>
       <c r="S28">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:20">
-      <c r="A29">
+      <c r="U28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21">
+      <c r="A29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29">
         <v>141</v>
       </c>
-      <c r="B29">
+      <c r="C29">
         <v>102</v>
       </c>
-      <c r="C29">
+      <c r="D29">
         <v>11</v>
       </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
       <c r="E29">
         <v>0</v>
       </c>
@@ -1984,17 +2217,17 @@
         <v>0</v>
       </c>
       <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
         <v>73</v>
       </c>
-      <c r="J29">
+      <c r="K29">
         <v>50</v>
       </c>
-      <c r="K29">
+      <c r="L29">
         <v>36</v>
       </c>
-      <c r="L29">
-        <v>0</v>
-      </c>
       <c r="M29">
         <v>0</v>
       </c>
@@ -2005,55 +2238,58 @@
         <v>0</v>
       </c>
       <c r="P29">
+        <v>0</v>
+      </c>
+      <c r="Q29">
         <v>11</v>
       </c>
-      <c r="Q29">
+      <c r="R29">
         <v>52</v>
       </c>
-      <c r="R29">
+      <c r="S29">
         <v>27</v>
       </c>
-      <c r="S29">
+      <c r="T29">
         <v>16</v>
       </c>
-      <c r="T29">
+      <c r="U29">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:20">
-      <c r="A30">
+    <row r="30" spans="1:21">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30">
         <v>60</v>
       </c>
-      <c r="B30">
-        <v>3</v>
-      </c>
       <c r="C30">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30">
         <v>0</v>
       </c>
       <c r="F30">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
         <v>7</v>
       </c>
-      <c r="I30">
+      <c r="J30">
         <v>164</v>
       </c>
-      <c r="J30">
+      <c r="K30">
         <v>43</v>
       </c>
-      <c r="K30">
-        <v>0</v>
-      </c>
       <c r="L30">
         <v>0</v>
       </c>
@@ -2067,24 +2303,27 @@
         <v>0</v>
       </c>
       <c r="P30">
+        <v>0</v>
+      </c>
+      <c r="Q30">
         <v>7</v>
       </c>
-      <c r="Q30">
+      <c r="R30">
         <v>136</v>
       </c>
-      <c r="R30">
+      <c r="S30">
         <v>32</v>
       </c>
-      <c r="S30">
-        <v>2</v>
-      </c>
       <c r="T30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20">
-      <c r="A31">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="U30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21">
+      <c r="A31" t="s">
+        <v>28</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -2093,66 +2332,69 @@
         <v>1</v>
       </c>
       <c r="D31">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E31">
+        <v>3</v>
+      </c>
+      <c r="F31">
         <v>6</v>
       </c>
-      <c r="F31">
+      <c r="G31">
         <v>5</v>
       </c>
-      <c r="G31">
-        <v>2</v>
-      </c>
       <c r="H31">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
         <v>86</v>
       </c>
-      <c r="J31">
+      <c r="K31">
         <v>5</v>
       </c>
-      <c r="K31">
-        <v>0</v>
-      </c>
       <c r="L31">
         <v>0</v>
       </c>
       <c r="M31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P31">
+        <v>1</v>
+      </c>
+      <c r="Q31">
         <v>9</v>
       </c>
-      <c r="Q31">
+      <c r="R31">
         <v>199</v>
       </c>
-      <c r="R31">
-        <v>1</v>
-      </c>
       <c r="S31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:20">
-      <c r="A32">
-        <v>1</v>
+      <c r="U31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21">
+      <c r="A32" t="s">
+        <v>29</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -2161,22 +2403,22 @@
         <v>0</v>
       </c>
       <c r="F32">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G32">
+        <v>2</v>
+      </c>
+      <c r="H32">
         <v>5</v>
       </c>
-      <c r="H32">
-        <v>1</v>
-      </c>
       <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="J32">
         <v>100</v>
       </c>
-      <c r="J32">
-        <v>2</v>
-      </c>
       <c r="K32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L32">
         <v>0</v>
@@ -2185,61 +2427,64 @@
         <v>0</v>
       </c>
       <c r="N32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P32">
+        <v>2</v>
+      </c>
+      <c r="Q32">
         <v>11</v>
       </c>
-      <c r="Q32">
+      <c r="R32">
         <v>182</v>
       </c>
-      <c r="R32">
-        <v>0</v>
-      </c>
       <c r="S32">
         <v>0</v>
       </c>
       <c r="T32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:20">
-      <c r="A33">
+      <c r="U32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21">
+      <c r="A33" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33">
         <v>60</v>
       </c>
-      <c r="B33">
+      <c r="C33">
         <v>8</v>
       </c>
-      <c r="C33">
-        <v>3</v>
-      </c>
       <c r="D33">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F33">
         <v>0</v>
       </c>
       <c r="G33">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H33">
+        <v>2</v>
+      </c>
+      <c r="I33">
         <v>5</v>
       </c>
-      <c r="I33">
+      <c r="J33">
         <v>197</v>
       </c>
-      <c r="J33">
+      <c r="K33">
         <v>40</v>
       </c>
-      <c r="K33">
-        <v>0</v>
-      </c>
       <c r="L33">
         <v>0</v>
       </c>
@@ -2253,52 +2498,55 @@
         <v>0</v>
       </c>
       <c r="P33">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q33">
+        <v>2</v>
+      </c>
+      <c r="R33">
         <v>127</v>
       </c>
-      <c r="R33">
+      <c r="S33">
         <v>19</v>
       </c>
-      <c r="S33">
-        <v>1</v>
-      </c>
       <c r="T33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20">
-      <c r="A34">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="U33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21">
+      <c r="A34" t="s">
+        <v>31</v>
       </c>
       <c r="B34">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C34">
         <v>3</v>
       </c>
       <c r="D34">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F34">
         <v>0</v>
       </c>
       <c r="G34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H34">
         <v>1</v>
       </c>
       <c r="I34">
+        <v>1</v>
+      </c>
+      <c r="J34">
         <v>26</v>
       </c>
-      <c r="J34">
-        <v>1</v>
-      </c>
       <c r="K34">
         <v>1</v>
       </c>
@@ -2306,39 +2554,42 @@
         <v>1</v>
       </c>
       <c r="M34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N34">
         <v>0</v>
       </c>
       <c r="O34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P34">
+        <v>1</v>
+      </c>
+      <c r="Q34">
         <v>22</v>
       </c>
-      <c r="Q34">
+      <c r="R34">
         <v>137</v>
       </c>
-      <c r="R34">
-        <v>0</v>
-      </c>
       <c r="S34">
         <v>0</v>
       </c>
       <c r="T34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:20">
-      <c r="A35">
+      <c r="U34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21">
+      <c r="A35" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35">
         <v>4</v>
       </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
       <c r="C35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -2350,17 +2601,17 @@
         <v>0</v>
       </c>
       <c r="G35">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H35">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I35">
+        <v>3</v>
+      </c>
+      <c r="J35">
         <v>75</v>
       </c>
-      <c r="J35">
-        <v>0</v>
-      </c>
       <c r="K35">
         <v>0</v>
       </c>
@@ -2377,158 +2628,167 @@
         <v>0</v>
       </c>
       <c r="P35">
+        <v>0</v>
+      </c>
+      <c r="Q35">
         <v>27</v>
       </c>
-      <c r="Q35">
+      <c r="R35">
         <v>160</v>
       </c>
-      <c r="R35">
-        <v>3</v>
-      </c>
       <c r="S35">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T35">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:20">
-      <c r="A36">
+        <v>2</v>
+      </c>
+      <c r="U35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21">
+      <c r="A36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36">
         <v>8</v>
       </c>
-      <c r="B36">
+      <c r="C36">
         <v>17</v>
       </c>
-      <c r="C36">
+      <c r="D36">
         <v>20</v>
       </c>
-      <c r="D36">
+      <c r="E36">
         <v>33</v>
       </c>
-      <c r="E36">
+      <c r="F36">
         <v>100</v>
       </c>
-      <c r="F36">
+      <c r="G36">
         <v>43</v>
       </c>
-      <c r="G36">
+      <c r="H36">
         <v>5</v>
       </c>
-      <c r="H36">
+      <c r="I36">
         <v>20</v>
       </c>
-      <c r="I36">
+      <c r="J36">
         <v>135</v>
       </c>
-      <c r="J36">
+      <c r="K36">
         <v>4</v>
       </c>
-      <c r="K36">
-        <v>0</v>
-      </c>
       <c r="L36">
         <v>0</v>
       </c>
       <c r="M36">
+        <v>0</v>
+      </c>
+      <c r="N36">
         <v>52</v>
       </c>
-      <c r="N36">
+      <c r="O36">
         <v>142</v>
       </c>
-      <c r="O36">
+      <c r="P36">
         <v>26</v>
       </c>
-      <c r="P36">
+      <c r="Q36">
         <v>44</v>
       </c>
-      <c r="Q36">
+      <c r="R36">
         <v>142</v>
       </c>
-      <c r="R36">
+      <c r="S36">
         <v>52</v>
       </c>
-      <c r="S36">
-        <v>0</v>
-      </c>
       <c r="T36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:20">
-      <c r="A37">
+      <c r="U36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21">
+      <c r="A37" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37">
         <v>68</v>
       </c>
-      <c r="B37">
+      <c r="C37">
         <v>105</v>
       </c>
-      <c r="C37">
+      <c r="D37">
         <v>21</v>
       </c>
-      <c r="D37">
+      <c r="E37">
         <v>52</v>
       </c>
-      <c r="E37">
+      <c r="F37">
         <v>35</v>
       </c>
-      <c r="F37">
+      <c r="G37">
         <v>7</v>
       </c>
-      <c r="G37">
-        <v>0</v>
-      </c>
       <c r="H37">
         <v>0</v>
       </c>
       <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37">
         <v>14</v>
       </c>
-      <c r="J37">
+      <c r="K37">
         <v>66</v>
       </c>
-      <c r="K37">
+      <c r="L37">
         <v>29</v>
       </c>
-      <c r="L37">
+      <c r="M37">
         <v>105</v>
       </c>
-      <c r="M37">
+      <c r="N37">
         <v>99</v>
       </c>
-      <c r="N37">
+      <c r="O37">
         <v>53</v>
       </c>
-      <c r="O37">
+      <c r="P37">
         <v>38</v>
       </c>
-      <c r="P37">
+      <c r="Q37">
         <v>15</v>
       </c>
-      <c r="Q37">
+      <c r="R37">
         <v>124</v>
       </c>
-      <c r="R37">
+      <c r="S37">
         <v>107</v>
       </c>
-      <c r="S37">
+      <c r="T37">
         <v>27</v>
       </c>
-      <c r="T37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20">
-      <c r="A38">
+      <c r="U37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21">
+      <c r="A38" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38">
         <v>46</v>
       </c>
-      <c r="B38">
+      <c r="C38">
         <v>16</v>
       </c>
-      <c r="C38">
+      <c r="D38">
         <v>4</v>
       </c>
-      <c r="D38">
-        <v>0</v>
-      </c>
       <c r="E38">
         <v>0</v>
       </c>
@@ -2542,14 +2802,14 @@
         <v>0</v>
       </c>
       <c r="I38">
+        <v>0</v>
+      </c>
+      <c r="J38">
         <v>193</v>
       </c>
-      <c r="J38">
+      <c r="K38">
         <v>30</v>
       </c>
-      <c r="K38">
-        <v>0</v>
-      </c>
       <c r="L38">
         <v>0</v>
       </c>
@@ -2566,27 +2826,30 @@
         <v>0</v>
       </c>
       <c r="Q38">
+        <v>0</v>
+      </c>
+      <c r="R38">
         <v>118</v>
       </c>
-      <c r="R38">
+      <c r="S38">
         <v>9</v>
       </c>
-      <c r="S38">
-        <v>1</v>
-      </c>
       <c r="T38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20">
-      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="U38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21">
+      <c r="A39" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39">
         <v>52</v>
       </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
       <c r="C39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D39">
         <v>0</v>
@@ -2598,19 +2861,19 @@
         <v>0</v>
       </c>
       <c r="G39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H39">
+        <v>1</v>
+      </c>
+      <c r="I39">
         <v>4</v>
       </c>
-      <c r="I39">
+      <c r="J39">
         <v>199</v>
       </c>
-      <c r="J39">
-        <v>1</v>
-      </c>
       <c r="K39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L39">
         <v>0</v>
@@ -2625,33 +2888,36 @@
         <v>0</v>
       </c>
       <c r="P39">
+        <v>0</v>
+      </c>
+      <c r="Q39">
         <v>22</v>
       </c>
-      <c r="Q39">
+      <c r="R39">
         <v>142</v>
       </c>
-      <c r="R39">
+      <c r="S39">
         <v>5</v>
       </c>
-      <c r="S39">
-        <v>0</v>
-      </c>
       <c r="T39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:20">
-      <c r="A40">
+      <c r="U39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21">
+      <c r="A40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40">
         <v>64</v>
       </c>
-      <c r="B40">
-        <v>2</v>
-      </c>
       <c r="C40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40">
         <v>0</v>
@@ -2663,17 +2929,17 @@
         <v>0</v>
       </c>
       <c r="H40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I40">
+        <v>1</v>
+      </c>
+      <c r="J40">
         <v>200</v>
       </c>
-      <c r="J40">
+      <c r="K40">
         <v>4</v>
       </c>
-      <c r="K40">
-        <v>0</v>
-      </c>
       <c r="L40">
         <v>0</v>
       </c>
@@ -2687,36 +2953,39 @@
         <v>0</v>
       </c>
       <c r="P40">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Q40">
+        <v>3</v>
+      </c>
+      <c r="R40">
         <v>117</v>
       </c>
-      <c r="R40">
-        <v>2</v>
-      </c>
       <c r="S40">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:20">
-      <c r="A41">
+      <c r="U40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21">
+      <c r="A41" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41">
         <v>57</v>
       </c>
-      <c r="B41">
+      <c r="C41">
         <v>9</v>
       </c>
-      <c r="C41">
-        <v>2</v>
-      </c>
       <c r="D41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F41">
         <v>0</v>
@@ -2728,14 +2997,14 @@
         <v>0</v>
       </c>
       <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41">
         <v>210</v>
       </c>
-      <c r="J41">
+      <c r="K41">
         <v>29</v>
       </c>
-      <c r="K41">
-        <v>0</v>
-      </c>
       <c r="L41">
         <v>0</v>
       </c>
@@ -2749,72 +3018,75 @@
         <v>0</v>
       </c>
       <c r="P41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q41">
+        <v>1</v>
+      </c>
+      <c r="R41">
         <v>89</v>
       </c>
-      <c r="R41">
+      <c r="S41">
         <v>11</v>
       </c>
-      <c r="S41">
-        <v>2</v>
-      </c>
       <c r="T41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:20">
-      <c r="A42">
+        <v>2</v>
+      </c>
+      <c r="U41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21">
+      <c r="A42" t="s">
+        <v>39</v>
+      </c>
+      <c r="B42">
         <v>4</v>
       </c>
-      <c r="B42">
+      <c r="C42">
         <v>34</v>
       </c>
-      <c r="C42">
+      <c r="D42">
         <v>30</v>
       </c>
-      <c r="D42">
+      <c r="E42">
         <v>27</v>
       </c>
-      <c r="E42">
+      <c r="F42">
         <v>121</v>
       </c>
-      <c r="F42">
+      <c r="G42">
         <v>12</v>
       </c>
-      <c r="G42">
-        <v>0</v>
-      </c>
       <c r="H42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J42">
         <v>0</v>
       </c>
       <c r="K42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L42">
+        <v>1</v>
+      </c>
+      <c r="M42">
         <v>24</v>
       </c>
-      <c r="M42">
+      <c r="N42">
         <v>135</v>
       </c>
-      <c r="N42">
+      <c r="O42">
         <v>26</v>
       </c>
-      <c r="O42">
+      <c r="P42">
         <v>10</v>
       </c>
-      <c r="P42">
-        <v>1</v>
-      </c>
       <c r="Q42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R42">
         <v>0</v>
@@ -2823,43 +3095,46 @@
         <v>0</v>
       </c>
       <c r="T42">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:20">
-      <c r="A43">
+        <v>0</v>
+      </c>
+      <c r="U42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21">
+      <c r="A43" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43">
         <v>137</v>
       </c>
-      <c r="B43">
+      <c r="C43">
         <v>24</v>
       </c>
-      <c r="C43">
-        <v>0</v>
-      </c>
       <c r="D43">
         <v>0</v>
       </c>
       <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
         <v>27</v>
       </c>
-      <c r="F43">
+      <c r="G43">
         <v>36</v>
       </c>
-      <c r="G43">
+      <c r="H43">
         <v>18</v>
       </c>
-      <c r="H43">
+      <c r="I43">
         <v>28</v>
       </c>
-      <c r="I43">
+      <c r="J43">
         <v>178</v>
       </c>
-      <c r="J43">
+      <c r="K43">
         <v>93</v>
       </c>
-      <c r="K43">
-        <v>0</v>
-      </c>
       <c r="L43">
         <v>0</v>
       </c>
@@ -2870,89 +3145,95 @@
         <v>0</v>
       </c>
       <c r="O43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P43">
+        <v>1</v>
+      </c>
+      <c r="Q43">
         <v>12</v>
       </c>
-      <c r="Q43">
+      <c r="R43">
         <v>62</v>
       </c>
-      <c r="R43">
+      <c r="S43">
         <v>31</v>
       </c>
-      <c r="S43">
-        <v>1</v>
-      </c>
       <c r="T43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:20">
-      <c r="A44">
+      <c r="U43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21">
+      <c r="A44" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44">
         <v>29</v>
       </c>
-      <c r="B44">
+      <c r="C44">
         <v>14</v>
       </c>
-      <c r="C44">
+      <c r="D44">
         <v>10</v>
       </c>
-      <c r="D44">
+      <c r="E44">
         <v>9</v>
       </c>
-      <c r="E44">
+      <c r="F44">
         <v>65</v>
       </c>
-      <c r="F44">
+      <c r="G44">
         <v>51</v>
       </c>
-      <c r="G44">
+      <c r="H44">
         <v>17</v>
       </c>
-      <c r="H44">
+      <c r="I44">
         <v>18</v>
       </c>
-      <c r="I44">
+      <c r="J44">
         <v>55</v>
       </c>
-      <c r="J44">
+      <c r="K44">
         <v>57</v>
       </c>
-      <c r="K44">
+      <c r="L44">
         <v>48</v>
       </c>
-      <c r="L44">
+      <c r="M44">
         <v>11</v>
       </c>
-      <c r="M44">
-        <v>3</v>
-      </c>
       <c r="N44">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O44">
+        <v>1</v>
+      </c>
+      <c r="P44">
         <v>14</v>
       </c>
-      <c r="P44">
+      <c r="Q44">
         <v>51</v>
       </c>
-      <c r="Q44">
+      <c r="R44">
         <v>24</v>
       </c>
-      <c r="R44">
+      <c r="S44">
         <v>38</v>
       </c>
-      <c r="S44">
+      <c r="T44">
         <v>55</v>
       </c>
-      <c r="T44">
+      <c r="U44">
         <v>116</v>
       </c>
     </row>
-    <row r="45" spans="1:20">
-      <c r="A45">
-        <v>0</v>
+    <row r="45" spans="1:21">
+      <c r="A45" t="s">
+        <v>42</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -2964,57 +3245,60 @@
         <v>0</v>
       </c>
       <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
         <v>68</v>
       </c>
-      <c r="F45">
+      <c r="G45">
         <v>52</v>
       </c>
-      <c r="G45">
-        <v>0</v>
-      </c>
       <c r="H45">
         <v>0</v>
       </c>
       <c r="I45">
+        <v>0</v>
+      </c>
+      <c r="J45">
         <v>127</v>
       </c>
-      <c r="J45">
+      <c r="K45">
         <v>12</v>
       </c>
-      <c r="K45">
-        <v>0</v>
-      </c>
       <c r="L45">
         <v>0</v>
       </c>
       <c r="M45">
+        <v>0</v>
+      </c>
+      <c r="N45">
         <v>39</v>
       </c>
-      <c r="N45">
+      <c r="O45">
         <v>21</v>
       </c>
-      <c r="O45">
-        <v>1</v>
-      </c>
       <c r="P45">
         <v>1</v>
       </c>
       <c r="Q45">
+        <v>1</v>
+      </c>
+      <c r="R45">
         <v>168</v>
       </c>
-      <c r="R45">
+      <c r="S45">
         <v>91</v>
       </c>
-      <c r="S45">
+      <c r="T45">
         <v>8</v>
       </c>
-      <c r="T45">
+      <c r="U45">
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:20">
-      <c r="A46">
-        <v>0</v>
+    <row r="46" spans="1:21">
+      <c r="A46" t="s">
+        <v>43</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -3026,23 +3310,23 @@
         <v>0</v>
       </c>
       <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
         <v>58</v>
       </c>
-      <c r="F46">
+      <c r="G46">
         <v>34</v>
       </c>
-      <c r="G46">
-        <v>0</v>
-      </c>
       <c r="H46">
         <v>0</v>
       </c>
       <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46">
         <v>34</v>
       </c>
-      <c r="J46">
-        <v>0</v>
-      </c>
       <c r="K46">
         <v>0</v>
       </c>
@@ -3050,33 +3334,36 @@
         <v>0</v>
       </c>
       <c r="M46">
+        <v>0</v>
+      </c>
+      <c r="N46">
         <v>56</v>
       </c>
-      <c r="N46">
+      <c r="O46">
         <v>32</v>
       </c>
-      <c r="O46">
+      <c r="P46">
         <v>7</v>
       </c>
-      <c r="P46">
+      <c r="Q46">
         <v>16</v>
       </c>
-      <c r="Q46">
+      <c r="R46">
         <v>50</v>
       </c>
-      <c r="R46">
-        <v>0</v>
-      </c>
       <c r="S46">
         <v>0</v>
       </c>
       <c r="T46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:20">
-      <c r="A47">
-        <v>0</v>
+      <c r="U46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21">
+      <c r="A47" t="s">
+        <v>44</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -3085,184 +3372,193 @@
         <v>0</v>
       </c>
       <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
         <v>4</v>
       </c>
-      <c r="E47">
+      <c r="F47">
         <v>31</v>
       </c>
-      <c r="F47">
+      <c r="G47">
         <v>5</v>
       </c>
-      <c r="G47">
-        <v>0</v>
-      </c>
       <c r="H47">
         <v>0</v>
       </c>
       <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47">
         <v>14</v>
       </c>
-      <c r="J47">
-        <v>0</v>
-      </c>
       <c r="K47">
         <v>0</v>
       </c>
       <c r="L47">
+        <v>0</v>
+      </c>
+      <c r="M47">
         <v>17</v>
       </c>
-      <c r="M47">
+      <c r="N47">
         <v>99</v>
       </c>
-      <c r="N47">
+      <c r="O47">
         <v>8</v>
       </c>
-      <c r="O47">
-        <v>2</v>
-      </c>
       <c r="P47">
+        <v>2</v>
+      </c>
+      <c r="Q47">
         <v>21</v>
       </c>
-      <c r="Q47">
+      <c r="R47">
         <v>77</v>
       </c>
-      <c r="R47">
-        <v>3</v>
-      </c>
       <c r="S47">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T47">
+        <v>0</v>
+      </c>
+      <c r="U47">
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:20">
-      <c r="A48">
+    <row r="48" spans="1:21">
+      <c r="A48" t="s">
+        <v>45</v>
+      </c>
+      <c r="B48">
         <v>5</v>
       </c>
-      <c r="B48">
+      <c r="C48">
         <v>16</v>
       </c>
-      <c r="C48">
+      <c r="D48">
         <v>20</v>
       </c>
-      <c r="D48">
+      <c r="E48">
         <v>62</v>
       </c>
-      <c r="E48">
+      <c r="F48">
         <v>150</v>
       </c>
-      <c r="F48">
+      <c r="G48">
         <v>10</v>
       </c>
-      <c r="G48">
-        <v>0</v>
-      </c>
       <c r="H48">
         <v>0</v>
       </c>
       <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48">
         <v>145</v>
       </c>
-      <c r="J48">
+      <c r="K48">
         <v>104</v>
       </c>
-      <c r="K48">
+      <c r="L48">
         <v>35</v>
       </c>
-      <c r="L48">
+      <c r="M48">
         <v>28</v>
       </c>
-      <c r="M48">
+      <c r="N48">
         <v>22</v>
       </c>
-      <c r="N48">
-        <v>0</v>
-      </c>
       <c r="O48">
         <v>0</v>
       </c>
       <c r="P48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q48">
+        <v>1</v>
+      </c>
+      <c r="R48">
         <v>73</v>
       </c>
-      <c r="R48">
+      <c r="S48">
         <v>43</v>
       </c>
-      <c r="S48">
+      <c r="T48">
         <v>8</v>
       </c>
-      <c r="T48">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:20">
-      <c r="A49">
-        <v>0</v>
+      <c r="U48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21">
+      <c r="A49" t="s">
+        <v>46</v>
       </c>
       <c r="B49">
         <v>0</v>
       </c>
       <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
         <v>7</v>
       </c>
-      <c r="D49">
+      <c r="E49">
         <v>17</v>
       </c>
-      <c r="E49">
+      <c r="F49">
         <v>5</v>
       </c>
-      <c r="F49">
-        <v>3</v>
-      </c>
       <c r="G49">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H49">
         <v>0</v>
       </c>
       <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="J49">
         <v>65</v>
       </c>
-      <c r="J49">
-        <v>2</v>
-      </c>
       <c r="K49">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L49">
+        <v>1</v>
+      </c>
+      <c r="M49">
         <v>11</v>
       </c>
-      <c r="M49">
+      <c r="N49">
         <v>8</v>
       </c>
-      <c r="N49">
-        <v>3</v>
-      </c>
       <c r="O49">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P49">
+        <v>0</v>
+      </c>
+      <c r="Q49">
         <v>31</v>
       </c>
-      <c r="Q49">
+      <c r="R49">
         <v>157</v>
       </c>
-      <c r="R49">
+      <c r="S49">
         <v>5</v>
       </c>
-      <c r="S49">
-        <v>0</v>
-      </c>
       <c r="T49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:20">
-      <c r="A50">
-        <v>0</v>
+      <c r="U49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21">
+      <c r="A50" t="s">
+        <v>47</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -3271,94 +3567,97 @@
         <v>0</v>
       </c>
       <c r="D50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50">
         <v>10</v>
       </c>
-      <c r="F50">
-        <v>2</v>
-      </c>
       <c r="G50">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H50">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I50">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K50">
         <v>0</v>
       </c>
       <c r="L50">
+        <v>0</v>
+      </c>
+      <c r="M50">
         <v>19</v>
       </c>
-      <c r="M50">
+      <c r="N50">
         <v>75</v>
       </c>
-      <c r="N50">
+      <c r="O50">
         <v>4</v>
       </c>
-      <c r="O50">
-        <v>3</v>
-      </c>
       <c r="P50">
+        <v>3</v>
+      </c>
+      <c r="Q50">
         <v>8</v>
       </c>
-      <c r="Q50">
+      <c r="R50">
         <v>22</v>
       </c>
-      <c r="R50">
-        <v>0</v>
-      </c>
       <c r="S50">
         <v>0</v>
       </c>
       <c r="T50">
+        <v>0</v>
+      </c>
+      <c r="U50">
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:20">
-      <c r="A51">
+    <row r="51" spans="1:21">
+      <c r="A51" t="s">
+        <v>48</v>
+      </c>
+      <c r="B51">
         <v>35</v>
       </c>
-      <c r="B51">
+      <c r="C51">
         <v>124</v>
       </c>
-      <c r="C51">
+      <c r="D51">
         <v>22</v>
       </c>
-      <c r="D51">
+      <c r="E51">
         <v>18</v>
       </c>
-      <c r="E51">
+      <c r="F51">
         <v>11</v>
       </c>
-      <c r="F51">
-        <v>1</v>
-      </c>
       <c r="G51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H51">
         <v>0</v>
       </c>
       <c r="I51">
+        <v>0</v>
+      </c>
+      <c r="J51">
         <v>21</v>
       </c>
-      <c r="J51">
+      <c r="K51">
         <v>86</v>
       </c>
-      <c r="K51">
+      <c r="L51">
         <v>30</v>
       </c>
-      <c r="L51">
-        <v>0</v>
-      </c>
       <c r="M51">
         <v>0</v>
       </c>
@@ -3369,24 +3668,27 @@
         <v>0</v>
       </c>
       <c r="P51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q51">
+        <v>1</v>
+      </c>
+      <c r="R51">
         <v>12</v>
       </c>
-      <c r="R51">
+      <c r="S51">
         <v>51</v>
       </c>
-      <c r="S51">
+      <c r="T51">
         <v>30</v>
       </c>
-      <c r="T51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:20">
-      <c r="A52">
-        <v>0</v>
+      <c r="U51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21">
+      <c r="A52" t="s">
+        <v>49</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -3395,54 +3697,57 @@
         <v>0</v>
       </c>
       <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
         <v>7</v>
       </c>
-      <c r="E52">
+      <c r="F52">
         <v>25</v>
       </c>
-      <c r="F52">
+      <c r="G52">
         <v>6</v>
       </c>
-      <c r="G52">
-        <v>1</v>
-      </c>
       <c r="H52">
         <v>1</v>
       </c>
       <c r="I52">
+        <v>1</v>
+      </c>
+      <c r="J52">
         <v>5</v>
       </c>
-      <c r="J52">
-        <v>1</v>
-      </c>
       <c r="K52">
+        <v>1</v>
+      </c>
+      <c r="L52">
         <v>4</v>
-      </c>
-      <c r="L52">
-        <v>5</v>
       </c>
       <c r="M52">
         <v>5</v>
       </c>
       <c r="N52">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O52">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P52">
+        <v>2</v>
+      </c>
+      <c r="Q52">
         <v>8</v>
       </c>
-      <c r="Q52">
+      <c r="R52">
         <v>22</v>
       </c>
-      <c r="R52">
-        <v>1</v>
-      </c>
       <c r="S52">
         <v>1</v>
       </c>
       <c r="T52">
+        <v>1</v>
+      </c>
+      <c r="U52">
         <v>2</v>
       </c>
     </row>

</xml_diff>